<commit_message>
colocando os graficos em escala
Signed-off-by: Jadson Santos <jadsonjs@gmail.com>
</commit_message>
<xml_diff>
--- a/MachineLearning/docs/data analysis.xlsx
+++ b/MachineLearning/docs/data analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KNN" sheetId="1" r:id="rId1"/>
@@ -1264,11 +1264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2105812568"/>
-        <c:axId val="2105804536"/>
+        <c:axId val="2063441240"/>
+        <c:axId val="2064508344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2105812568"/>
+        <c:axId val="2063441240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,12 +1296,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105804536"/>
+        <c:crossAx val="2064508344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2105804536"/>
+        <c:axId val="2064508344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1330,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105812568"/>
+        <c:crossAx val="2063441240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1551,11 +1551,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106848904"/>
-        <c:axId val="2106851880"/>
+        <c:axId val="2063923432"/>
+        <c:axId val="2063920440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106848904"/>
+        <c:axId val="2063923432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106851880"/>
+        <c:crossAx val="2063920440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1572,9 +1572,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106851880"/>
+        <c:axId val="2063920440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1583,7 +1584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106848904"/>
+        <c:crossAx val="2063923432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1805,11 +1806,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105498168"/>
-        <c:axId val="2105501144"/>
+        <c:axId val="2063502088"/>
+        <c:axId val="2063505064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105498168"/>
+        <c:axId val="2063502088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105501144"/>
+        <c:crossAx val="2063505064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +1827,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105501144"/>
+        <c:axId val="2063505064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,7 +1838,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105498168"/>
+        <c:crossAx val="2063502088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2059,11 +2060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2104545496"/>
-        <c:axId val="2104542504"/>
+        <c:axId val="2063533080"/>
+        <c:axId val="2063536056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104545496"/>
+        <c:axId val="2063533080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104542504"/>
+        <c:crossAx val="2063536056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2080,9 +2081,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104542504"/>
+        <c:axId val="2063536056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2091,7 +2093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104545496"/>
+        <c:crossAx val="2063533080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2313,11 +2315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2104515544"/>
-        <c:axId val="2104512552"/>
+        <c:axId val="2063563032"/>
+        <c:axId val="2063566008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104515544"/>
+        <c:axId val="2063563032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,7 +2328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104512552"/>
+        <c:crossAx val="2063566008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2334,9 +2336,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104512552"/>
+        <c:axId val="2063566008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2345,7 +2348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104515544"/>
+        <c:crossAx val="2063563032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2567,11 +2570,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106674856"/>
-        <c:axId val="2106677832"/>
+        <c:axId val="2062876520"/>
+        <c:axId val="2062873528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106674856"/>
+        <c:axId val="2062876520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106677832"/>
+        <c:crossAx val="2062873528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2588,7 +2591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106677832"/>
+        <c:axId val="2062873528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106674856"/>
+        <c:crossAx val="2062876520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2821,11 +2824,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106705528"/>
-        <c:axId val="2106708504"/>
+        <c:axId val="2062845896"/>
+        <c:axId val="2062842904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106705528"/>
+        <c:axId val="2062845896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106708504"/>
+        <c:crossAx val="2062842904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2842,7 +2845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106708504"/>
+        <c:axId val="2062842904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +2856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106705528"/>
+        <c:crossAx val="2062845896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3075,11 +3078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106735160"/>
-        <c:axId val="2106738136"/>
+        <c:axId val="2062816232"/>
+        <c:axId val="2062813240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106735160"/>
+        <c:axId val="2062816232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3088,7 +3091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106738136"/>
+        <c:crossAx val="2062813240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3096,7 +3099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106738136"/>
+        <c:axId val="2062813240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3107,7 +3110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106735160"/>
+        <c:crossAx val="2062816232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3329,11 +3332,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106787848"/>
-        <c:axId val="2106790824"/>
+        <c:axId val="2064603288"/>
+        <c:axId val="2064606264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106787848"/>
+        <c:axId val="2064603288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3342,7 +3345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106790824"/>
+        <c:crossAx val="2064606264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3350,7 +3353,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106790824"/>
+        <c:axId val="2064606264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3361,7 +3364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106787848"/>
+        <c:crossAx val="2064603288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3583,11 +3586,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106818568"/>
-        <c:axId val="2106821544"/>
+        <c:axId val="2063953864"/>
+        <c:axId val="2063950872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106818568"/>
+        <c:axId val="2063953864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3596,7 +3599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106821544"/>
+        <c:crossAx val="2063950872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3604,9 +3607,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106821544"/>
+        <c:axId val="2063950872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3615,7 +3619,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106818568"/>
+        <c:crossAx val="2063953864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3682,8 +3686,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
@@ -3712,8 +3716,8 @@
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1282700</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
@@ -3962,27 +3966,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="em-silhouettes" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="em-DBs" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="em-silhouettes" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-DBs" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-silhouettes_2" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-silhouettes_1" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-CRs" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-silhouettes_1" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-silhouettes_2" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kmeans-DBs" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3990,11 +3994,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="agglomerative-DBs_1" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="agglomerative-silhouettes_1" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="agglomerative-silhouettes_1" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="agglomerative-DBs_1" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4989,8 +4993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I332"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59:H77"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6777,8 +6781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C10:D79"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61:D79"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7283,8 +7287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55:H73"/>
+    <sheetView tabSelected="1" topLeftCell="D48" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8987,7 +8991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>

</xml_diff>